<commit_message>
End of section 3
</commit_message>
<xml_diff>
--- a/Angular Tips.xlsx
+++ b/Angular Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Entreprise Log Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B73EBF-03B6-42B2-A638-7551D3887DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE0FEEE-BABE-4FDE-8D01-DB20871844EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="8415" windowWidth="35985" windowHeight="23985" activeTab="3" xr2:uid="{6B65A01A-198D-464F-B188-B42A26C4F361}"/>
+    <workbookView xWindow="-15" yWindow="14520" windowWidth="35985" windowHeight="17880" activeTab="2" xr2:uid="{6B65A01A-198D-464F-B188-B42A26C4F361}"/>
   </bookViews>
   <sheets>
     <sheet name="Cmd" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="86">
   <si>
     <t>Description</t>
   </si>
@@ -226,13 +226,73 @@
   </si>
   <si>
     <t>Creation d'un fichier gitignore</t>
+  </si>
+  <si>
+    <t>git remote add origin https://github.com/Noburo-59/Tracker.git</t>
+  </si>
+  <si>
+    <t>Ajout du serveur</t>
+  </si>
+  <si>
+    <t>npm install -g @angular/cli</t>
+  </si>
+  <si>
+    <t>NPM</t>
+  </si>
+  <si>
+    <t>ng version</t>
+  </si>
+  <si>
+    <t>Dernière version</t>
+  </si>
+  <si>
+    <t>ng new client</t>
+  </si>
+  <si>
+    <t>npm -v</t>
+  </si>
+  <si>
+    <t>node -v</t>
+  </si>
+  <si>
+    <t>dotnet ef</t>
+  </si>
+  <si>
+    <t>VERSIONS</t>
+  </si>
+  <si>
+    <t>nvm -h</t>
+  </si>
+  <si>
+    <t>ng serve</t>
+  </si>
+  <si>
+    <t>Lance le client</t>
+  </si>
+  <si>
+    <t>Angular TypeScript Snippets</t>
+  </si>
+  <si>
+    <t>Angular Language Service</t>
+  </si>
+  <si>
+    <t>ng add ngx-bootstrap</t>
+  </si>
+  <si>
+    <t>npm install font-awesome</t>
+  </si>
+  <si>
+    <t>Font</t>
+  </si>
+  <si>
+    <t>Ngx Bootstraps</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,6 +332,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -299,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -311,6 +377,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988D6CB0-1A26-4388-9B71-F1A421880A05}">
-  <dimension ref="B2:C21"/>
+  <dimension ref="B2:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,57 +769,102 @@
       <c r="C11"/>
     </row>
     <row r="12" spans="2:3" s="1" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B12"/>
+      <c r="B12" t="s">
+        <v>80</v>
+      </c>
       <c r="C12"/>
     </row>
     <row r="13" spans="2:3" s="1" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13"/>
+    </row>
+    <row r="14" spans="2:3" s="1" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14"/>
+      <c r="C14"/>
+    </row>
+    <row r="15" spans="2:3" s="1" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>57</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="2:3" s="1" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B19" s="2" t="s">
+    <row r="21" spans="2:3" s="1" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" s="1" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -764,7 +878,7 @@
   <dimension ref="B2:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B73A759-8978-47CC-9409-DED03B2FE2BE}">
-  <dimension ref="B2:C5"/>
+  <dimension ref="B2:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,8 +1055,47 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+    </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
+      <c r="B5" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" t="s">
+        <v>84</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -952,10 +1105,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECC3ABA-C5C6-4B37-A192-E0C9F2625DF5}">
-  <dimension ref="B2:C12"/>
+  <dimension ref="B2:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,60 +1143,86 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
-    </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>47</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C16" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" s="1" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
End of section 4
</commit_message>
<xml_diff>
--- a/Angular Tips.xlsx
+++ b/Angular Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Entreprise Log Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE0FEEE-BABE-4FDE-8D01-DB20871844EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CC0E7B-DDBB-4FDA-B083-719383A7C621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="14520" windowWidth="35985" windowHeight="17880" activeTab="2" xr2:uid="{6B65A01A-198D-464F-B188-B42A26C4F361}"/>
+    <workbookView xWindow="-15" yWindow="14520" windowWidth="35985" windowHeight="17880" xr2:uid="{6B65A01A-198D-464F-B188-B42A26C4F361}"/>
   </bookViews>
   <sheets>
     <sheet name="Cmd" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="88">
   <si>
     <t>Description</t>
   </si>
@@ -286,6 +286,12 @@
   </si>
   <si>
     <t>Ngx Bootstraps</t>
+  </si>
+  <si>
+    <t>System.IdentityModel.Tokens.Jwt</t>
+  </si>
+  <si>
+    <t>Microsoft.AspNetCore.Authentication.JwtBearer</t>
   </si>
 </sst>
 </file>
@@ -694,15 +700,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988D6CB0-1A26-4388-9B71-F1A421880A05}">
-  <dimension ref="B2:C30"/>
+  <dimension ref="B2:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="145.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -834,36 +840,46 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="2:3" s="1" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B25" s="2" t="s">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" s="1" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B27" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1037,7 +1053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B73A759-8978-47CC-9409-DED03B2FE2BE}">
   <dimension ref="B2:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
end of section 5
</commit_message>
<xml_diff>
--- a/Angular Tips.xlsx
+++ b/Angular Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Entreprise Log Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CC0E7B-DDBB-4FDA-B083-719383A7C621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7447AC6D-AAA8-4180-8498-D046320EEBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="14520" windowWidth="35985" windowHeight="17880" xr2:uid="{6B65A01A-198D-464F-B188-B42A26C4F361}"/>
+    <workbookView xWindow="0" yWindow="14520" windowWidth="35985" windowHeight="17880" activeTab="2" xr2:uid="{6B65A01A-198D-464F-B188-B42A26C4F361}"/>
   </bookViews>
   <sheets>
     <sheet name="Cmd" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="99">
   <si>
     <t>Description</t>
   </si>
@@ -292,13 +292,380 @@
   </si>
   <si>
     <t>Microsoft.AspNetCore.Authentication.JwtBearer</t>
+  </si>
+  <si>
+    <t>ng g -h</t>
+  </si>
+  <si>
+    <t>List des génération angular possible</t>
+  </si>
+  <si>
+    <t>ng g c nav --skip-tests</t>
+  </si>
+  <si>
+    <t>Création d'un component sans test</t>
+  </si>
+  <si>
+    <t>Angular</t>
+  </si>
+  <si>
+    <t>#loginForm permet de transformer la form en angularform, (ngSubmit) est une directive pour soumettre</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>form</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#loginForm</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"ngForm"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>class</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"navbar-nav ms-auto mb-2 mb-lg-0"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ngSubmit</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>login</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF808080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>ng g s account</t>
+  </si>
+  <si>
+    <t>ajout d'un service</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>div</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> *</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ngIf</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>accountService</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.currentUser$ | </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>async</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>class</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"dropdown"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>dropdown</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF808080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Le pipe | async permet de désabonner directement l'observable currentUser$ du service account</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,6 +711,55 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF808080"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF569CD6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF9CDCFE"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FFDCDCAA"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -371,7 +787,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -386,6 +802,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,7 +1122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988D6CB0-1A26-4388-9B71-F1A421880A05}">
   <dimension ref="B2:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -1051,16 +1471,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B73A759-8978-47CC-9409-DED03B2FE2BE}">
-  <dimension ref="B2:C8"/>
+  <dimension ref="B2:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="55.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="85.28515625" customWidth="1"/>
+    <col min="2" max="2" width="116.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" s="1" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
@@ -1111,6 +1531,54 @@
       </c>
       <c r="C8" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" s="1" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
End of section 6
</commit_message>
<xml_diff>
--- a/Angular Tips.xlsx
+++ b/Angular Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Entreprise Log Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7447AC6D-AAA8-4180-8498-D046320EEBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D827CAF-866B-4BB6-84E2-E7F7B8C24B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="14520" windowWidth="35985" windowHeight="17880" activeTab="2" xr2:uid="{6B65A01A-198D-464F-B188-B42A26C4F361}"/>
+    <workbookView xWindow="135" yWindow="13920" windowWidth="28035" windowHeight="17880" activeTab="2" xr2:uid="{6B65A01A-198D-464F-B188-B42A26C4F361}"/>
   </bookViews>
   <sheets>
     <sheet name="Cmd" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="117">
   <si>
     <t>Description</t>
   </si>
@@ -659,6 +659,204 @@
   </si>
   <si>
     <t>Le pipe | async permet de désabonner directement l'observable currentUser$ du service account</t>
+  </si>
+  <si>
+    <t>npm install ngx-toastr</t>
+  </si>
+  <si>
+    <t>Ajout d'une librairie de popup angular</t>
+  </si>
+  <si>
+    <t>            ],</t>
+  </si>
+  <si>
+    <r>
+      <t> "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>styles</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>": [</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>              </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"./node_modules/ngx-bootstrap/datepicker/bs-datepicker.css"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>              </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"./node_modules/bootstrap/dist/css/bootstrap.min.css"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>              </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"./node_modules/font-awesome/css/font-awesome.css"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>              </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"./node_modules/ngx-toastr/toastr.css"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>              </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"src/styles.css"</t>
+    </r>
+  </si>
+  <si>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">angular.json, ajout des css </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ng g guard auth --skip-tests</t>
+  </si>
+  <si>
+    <t>Ajout d'un service de guard pour le routing</t>
+  </si>
+  <si>
+    <t>npm install bootswatch</t>
+  </si>
+  <si>
+    <t>Thème pour bootstrap</t>
+  </si>
+  <si>
+    <r>
+      <t>              </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"./node_modules/bootswatch/dist/united/bootstrap.css"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <t>ng g m shared --flat</t>
+  </si>
+  <si>
+    <t>Ajout d'un module de partage de librairie</t>
   </si>
 </sst>
 </file>
@@ -787,7 +985,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -806,6 +1004,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1471,10 +1672,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B73A759-8978-47CC-9409-DED03B2FE2BE}">
-  <dimension ref="B2:C16"/>
+  <dimension ref="B2:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,27 +1758,110 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="2:3" s="1" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B14" s="2" t="s">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" s="1" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B19" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B23" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B24" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B25" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B26" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" s="1" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B33" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B15" s="8" t="s">
+    <row r="34" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C34" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B16" s="8" t="s">
+    <row r="35" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B35" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C35" s="9" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>